<commit_message>
Atualizando a planilha de riscos e backlog
</commit_message>
<xml_diff>
--- a/Backlog-Orchis System.xlsx
+++ b/Backlog-Orchis System.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76E9D651-4BBB-4A36-B6D1-90841CCC0057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\OrchisSystems\Documentacao\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272AEB91-CDEE-47F9-833D-6B7E31527685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="150">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -60,9 +65,6 @@
     <t>TAMANHO (F)</t>
   </si>
   <si>
-    <t>ESTIMATIVA</t>
-  </si>
-  <si>
     <t>SPRINT</t>
   </si>
   <si>
@@ -84,9 +86,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>2 DIAS</t>
-  </si>
-  <si>
     <t>SP1</t>
   </si>
   <si>
@@ -99,9 +98,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>4 DIAS</t>
-  </si>
-  <si>
     <t>CONTEXTO</t>
   </si>
   <si>
@@ -111,9 +107,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>3 DIAS</t>
-  </si>
-  <si>
     <t>OBJETIVO</t>
   </si>
   <si>
@@ -123,9 +116,6 @@
     <t>PP</t>
   </si>
   <si>
-    <t>1 DIA</t>
-  </si>
-  <si>
     <t>JUSTIFICATIVA</t>
   </si>
   <si>
@@ -204,9 +194,6 @@
     <t>GG</t>
   </si>
   <si>
-    <t>5 DIAS</t>
-  </si>
-  <si>
     <t>CRIAÇÃO DO BANCO DE DADOS</t>
   </si>
   <si>
@@ -478,13 +465,34 @@
   </si>
   <si>
     <t>TABELAS FINAIS PARA O FUNCIONAMENTO EFETIVO DO SITE INSTITUCIONAL</t>
+  </si>
+  <si>
+    <t>Planejado</t>
+  </si>
+  <si>
+    <t>Realizado</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>SP01</t>
+  </si>
+  <si>
+    <t>SP03</t>
+  </si>
+  <si>
+    <t>SP02</t>
+  </si>
+  <si>
+    <t>ESTIMATIVA(Dias)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -669,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -699,6 +707,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,30 +876,29 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7910790715812902E-2"/>
+          <c:y val="0.10564822944103014"/>
+          <c:w val="0.94187406236338711"/>
+          <c:h val="0.76579008616021327"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>{"Sprint"}</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sprint</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -914,6 +931,27 @@
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>{"Sprint"}</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Sprint</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-634E-46AF-8092-3F11BAEB8FA8}"/>
             </c:ext>
@@ -971,7 +1009,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="774802440"/>
@@ -1030,7 +1068,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="774800392"/>
@@ -1072,7 +1110,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1102,12 +1140,438 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Backlog!$G$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planejado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Backlog!$F$59:$F$62</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SP01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SP02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SP03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Backlog!$G$59:$G$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE97-45CB-9F35-0EAB3744AF50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Backlog!$H$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Realizado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="63500" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Backlog!$F$59:$F$62</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SP01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SP02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SP03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Backlog!$H$59:$H$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE97-45CB-9F35-0EAB3744AF50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1500273727"/>
+        <c:axId val="1500270847"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1500273727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1500270847"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1500270847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1500273727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1153,7 +1617,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1702,6 +2722,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1269890</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>20045</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>418769</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>156045</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97CFAB57-5F99-08EE-A3B6-C469E4B001B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2755,46 +3811,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="W67" sqref="W67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="8.85546875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="41.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="1" customWidth="1"/>
+    <col min="11" max="14" width="8.88671875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" ht="25.5" customHeight="1">
+    <row r="2" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2819,1894 +3875,1950 @@
       <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="25.5" customHeight="1">
+    <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="10">
         <v>1</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H3" s="10">
         <v>5</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>17</v>
+      <c r="I3" s="15">
+        <v>2</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="42" customHeight="1">
+    <row r="4" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="10">
         <v>2</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="G4" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H4" s="10">
         <v>13</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>22</v>
+      <c r="I4" s="15">
+        <v>4</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="33.75" customHeight="1">
+    <row r="5" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="10">
         <v>3</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H5" s="10">
         <v>8</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>26</v>
+      <c r="I5" s="15">
+        <v>3</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="25.5" customHeight="1">
+    <row r="6" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="10">
         <v>12</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="G6" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H6" s="10">
         <v>3</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>30</v>
+      <c r="I6" s="15">
+        <v>1</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="25.5" customHeight="1">
+    <row r="7" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10">
         <v>13</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="G7" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7" s="10">
         <v>3</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>30</v>
+      <c r="I7" s="15">
+        <v>1</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" ht="25.5" customHeight="1">
+    <row r="8" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="10">
         <v>14</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H8" s="10">
         <v>5</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>17</v>
+      <c r="I8" s="15">
+        <v>2</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="25.5" customHeight="1">
+    <row r="9" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="10">
         <v>17</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H9" s="10">
         <v>5</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>17</v>
+      <c r="I9" s="15">
+        <v>2</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="10">
         <v>18</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H10" s="10">
         <v>5</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>17</v>
+      <c r="I10" s="15">
+        <v>2</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="48" customHeight="1">
+    <row r="11" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="10">
         <v>4</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" s="10">
         <v>8</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>26</v>
+      <c r="I11" s="15">
+        <v>3</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="26.25" customHeight="1">
+    <row r="12" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="10">
         <v>19</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H12" s="10">
         <v>5</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>17</v>
+      <c r="I12" s="15">
+        <v>2</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="25.5" customHeight="1">
+    <row r="13" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="10">
         <v>20</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H13" s="10">
         <v>5</v>
       </c>
-      <c r="I13" s="11" t="s">
-        <v>17</v>
+      <c r="I13" s="15">
+        <v>2</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="35.25" customHeight="1">
+    <row r="14" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D14" s="10">
         <v>21</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H14" s="10">
         <v>8</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>26</v>
+      <c r="I14" s="15">
+        <v>3</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" ht="39" customHeight="1">
+    <row r="15" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="10">
         <v>5</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H15" s="10">
         <v>8</v>
       </c>
-      <c r="I15" s="11" t="s">
-        <v>26</v>
+      <c r="I15" s="15">
+        <v>3</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="25.5" customHeight="1">
+    <row r="16" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="10">
         <v>6</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H16" s="10">
         <v>21</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>57</v>
+      <c r="I16" s="15">
+        <v>5</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="39" customHeight="1">
+    <row r="17" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="10">
         <v>7</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H17" s="10">
         <v>3</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>30</v>
+      <c r="I17" s="15">
+        <v>1</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="39" customHeight="1">
+    <row r="18" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="10">
         <v>8</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H18" s="10">
         <v>8</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>26</v>
+      <c r="I18" s="15">
+        <v>3</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" ht="25.5" customHeight="1">
+    <row r="19" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="10">
         <v>9</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H19" s="10">
         <v>8</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>26</v>
+      <c r="I19" s="15">
+        <v>3</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="39.75" customHeight="1">
+    <row r="20" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="10">
         <v>15</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H20" s="10">
         <v>5</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>17</v>
+      <c r="I20" s="15">
+        <v>2</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="39" customHeight="1">
+    <row r="21" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="10">
         <v>16</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H21" s="10">
         <v>5</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>17</v>
+      <c r="I21" s="15">
+        <v>2</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="25.5" customHeight="1">
+    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="10">
         <v>22</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H22" s="10">
         <v>8</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>26</v>
+      <c r="I22" s="15">
+        <v>3</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" ht="24.75" customHeight="1">
+    <row r="23" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="10">
         <v>10</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H23" s="10">
         <v>3</v>
       </c>
-      <c r="I23" s="11" t="s">
-        <v>30</v>
+      <c r="I23" s="15">
+        <v>1</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="25.5" customHeight="1">
+    <row r="24" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="10">
         <v>11</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H24" s="10">
         <v>3</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>30</v>
+      <c r="I24" s="15">
+        <v>1</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="25.5" customHeight="1">
+    <row r="25" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="10">
         <v>16</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H25" s="10">
         <v>3</v>
       </c>
-      <c r="I25" s="11" t="s">
-        <v>30</v>
+      <c r="I25" s="15">
+        <v>1</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K25" s="13"/>
       <c r="L25" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="M25" s="10">
         <f>SUM(M27:M28)</f>
         <v>322</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="35.25" customHeight="1">
+    <row r="26" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="10">
         <v>1</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26" s="10">
         <v>5</v>
       </c>
-      <c r="I26" s="11" t="s">
-        <v>17</v>
+      <c r="I26" s="15">
+        <v>2</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K26" s="13"/>
       <c r="L26" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M26" s="10">
         <f>SUMIF(J3:J24,"SP1",H3:H24)</f>
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="25.5" customHeight="1">
+    <row r="27" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="10">
         <v>11</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H27" s="10">
         <v>13</v>
       </c>
-      <c r="I27" s="11" t="s">
-        <v>22</v>
+      <c r="I27" s="15">
+        <v>4</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K27" s="13"/>
       <c r="L27" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M27" s="10">
         <f>SUMIF(J25:J55,"SP2",H25:H55)</f>
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="25.5" customHeight="1">
+    <row r="28" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="10">
         <v>10</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H28" s="10">
         <v>8</v>
       </c>
-      <c r="I28" s="11" t="s">
-        <v>26</v>
+      <c r="I28" s="15">
+        <v>3</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K28" s="13"/>
       <c r="L28" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="M28" s="10">
         <f>SUMIF(J41:J55,"SP3",H41:H55)</f>
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="24.75" customHeight="1">
+    <row r="29" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" s="10">
         <v>3</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H29" s="10">
         <v>21</v>
       </c>
-      <c r="I29" s="11" t="s">
-        <v>57</v>
+      <c r="I29" s="15">
+        <v>5</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K29" s="13"/>
       <c r="L29" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M29" s="10">
-        <v>155.66999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="25.5" customHeight="1">
+        <f>(M26+M27+M28)/3</f>
+        <v>155.66666666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" s="10">
         <v>4</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H30" s="10">
         <v>13</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>22</v>
+      <c r="I30" s="15">
+        <v>4</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
     </row>
-    <row r="31" spans="1:13" ht="25.5" customHeight="1">
+    <row r="31" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" s="10">
         <v>5</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H31" s="10">
         <v>21</v>
       </c>
-      <c r="I31" s="11" t="s">
-        <v>57</v>
+      <c r="I31" s="15">
+        <v>5</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="39" customHeight="1">
+    <row r="32" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="10">
         <v>9</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H32" s="10">
         <v>8</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>26</v>
+      <c r="I32" s="15">
+        <v>3</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" ht="25.5" customHeight="1">
+    <row r="33" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="10">
         <v>8</v>
       </c>
       <c r="E33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="G33" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H33" s="10">
         <v>3</v>
       </c>
-      <c r="I33" s="11" t="s">
-        <v>30</v>
+      <c r="I33" s="15">
+        <v>1</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="37.5" customHeight="1">
+    <row r="34" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="10">
         <v>2</v>
       </c>
       <c r="E34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H34" s="10">
         <v>5</v>
       </c>
-      <c r="I34" s="11" t="s">
-        <v>17</v>
+      <c r="I34" s="15">
+        <v>2</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="25.5" customHeight="1">
+    <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" s="10">
         <v>6</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H35" s="10">
         <v>5</v>
       </c>
-      <c r="I35" s="11" t="s">
-        <v>17</v>
+      <c r="I35" s="15">
+        <v>2</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="25.5" customHeight="1">
+    <row r="36" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" s="10">
         <v>7</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H36" s="10">
         <v>8</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>26</v>
+      <c r="I36" s="15">
+        <v>3</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="25.5" customHeight="1">
+    <row r="37" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="10">
         <v>13</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H37" s="10">
         <v>13</v>
       </c>
-      <c r="I37" s="11" t="s">
-        <v>22</v>
+      <c r="I37" s="15">
+        <v>4</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="25.5" customHeight="1">
+    <row r="38" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" s="10">
         <v>12</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H38" s="10">
         <v>13</v>
       </c>
-      <c r="I38" s="11" t="s">
-        <v>22</v>
+      <c r="I38" s="15">
+        <v>4</v>
       </c>
       <c r="J38" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" ht="39" customHeight="1">
+    <row r="39" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D39" s="10">
         <v>14</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H39" s="10">
         <v>8</v>
       </c>
-      <c r="I39" s="11" t="s">
-        <v>26</v>
+      <c r="I39" s="15">
+        <v>3</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="25.5" customHeight="1">
+    <row r="40" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="10">
         <v>15</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H40" s="10">
         <v>8</v>
       </c>
-      <c r="I40" s="11" t="s">
-        <v>26</v>
+      <c r="I40" s="15">
+        <v>3</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" ht="25.35" customHeight="1">
+    <row r="41" spans="1:13" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41" s="10">
         <v>12</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H41" s="10">
         <v>13</v>
       </c>
-      <c r="I41" s="11" t="s">
-        <v>22</v>
+      <c r="I41" s="15">
+        <v>4</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="27.95" customHeight="1">
+    <row r="42" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42" s="10">
         <v>3</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H42" s="10">
         <v>21</v>
       </c>
-      <c r="I42" s="11" t="s">
-        <v>57</v>
+      <c r="I42" s="15">
+        <v>5</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" ht="27.4" customHeight="1">
+    <row r="43" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43" s="10">
         <v>13</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H43" s="10">
         <v>8</v>
       </c>
-      <c r="I43" s="11" t="s">
-        <v>26</v>
+      <c r="I43" s="15">
+        <v>3</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" ht="29.65" customHeight="1">
+    <row r="44" spans="1:13" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44" s="10">
         <v>5</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H44" s="10">
         <v>5</v>
       </c>
-      <c r="I44" s="11" t="s">
-        <v>17</v>
+      <c r="I44" s="15">
+        <v>2</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" ht="27.95" customHeight="1">
+    <row r="45" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D45" s="10">
         <v>4</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H45" s="10">
         <v>5</v>
       </c>
-      <c r="I45" s="11" t="s">
-        <v>17</v>
+      <c r="I45" s="15">
+        <v>2</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" ht="27.95" customHeight="1">
+    <row r="46" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D46" s="10">
         <v>11</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H46" s="10">
         <v>13</v>
       </c>
-      <c r="I46" s="11" t="s">
-        <v>22</v>
+      <c r="I46" s="15">
+        <v>4</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" ht="27.95" customHeight="1">
+    <row r="47" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47" s="10">
         <v>10</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H47" s="10">
         <v>8</v>
       </c>
-      <c r="I47" s="11" t="s">
-        <v>26</v>
+      <c r="I47" s="15">
+        <v>3</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" ht="25.5" customHeight="1">
+    <row r="48" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D48" s="10">
         <v>9</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H48" s="10">
         <v>8</v>
       </c>
-      <c r="I48" s="11" t="s">
-        <v>26</v>
+      <c r="I48" s="15">
+        <v>3</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" ht="27.95" customHeight="1">
+    <row r="49" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D49" s="10">
         <v>8</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H49" s="10">
         <v>13</v>
       </c>
-      <c r="I49" s="11" t="s">
-        <v>22</v>
+      <c r="I49" s="15">
+        <v>4</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="25.35" customHeight="1">
+    <row r="50" spans="1:13" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="10">
         <v>15</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H50" s="10">
         <v>5</v>
       </c>
-      <c r="I50" s="11" t="s">
-        <v>17</v>
+      <c r="I50" s="15">
+        <v>2</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" ht="27.95" customHeight="1">
+    <row r="51" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D51" s="10">
         <v>14</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="10">
         <v>5</v>
       </c>
-      <c r="I51" s="11" t="s">
-        <v>17</v>
+      <c r="I51" s="15">
+        <v>2</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="36.75" customHeight="1">
+    <row r="52" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D52" s="10">
         <v>7</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H52" s="10">
         <v>21</v>
       </c>
-      <c r="I52" s="11" t="s">
-        <v>57</v>
+      <c r="I52" s="15">
+        <v>5</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" ht="27.95" customHeight="1">
+    <row r="53" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D53" s="10">
         <v>1</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H53" s="10">
         <v>21</v>
       </c>
-      <c r="I53" s="11" t="s">
-        <v>57</v>
+      <c r="I53" s="15">
+        <v>5</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" ht="27.95" customHeight="1">
+    <row r="54" spans="1:13" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54" s="10">
         <v>2</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H54" s="10">
         <v>13</v>
       </c>
-      <c r="I54" s="11" t="s">
-        <v>22</v>
+      <c r="I54" s="15">
+        <v>4</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" ht="39.75" customHeight="1">
+    <row r="55" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D55" s="10">
         <v>6</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H55" s="10">
         <v>8</v>
       </c>
-      <c r="I55" s="11" t="s">
-        <v>26</v>
+      <c r="I55" s="15">
+        <v>3</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K55" s="2"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
+    </row>
+    <row r="58" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G58" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F59" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G59" s="1">
+        <v>53</v>
+      </c>
+      <c r="H59" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G60" s="1">
+        <f>G59-22</f>
+        <v>31</v>
+      </c>
+      <c r="H60" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G61" s="1">
+        <f>G60-16</f>
+        <v>15</v>
+      </c>
+      <c r="H61" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G62" s="1">
+        <f>G61-15</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Atualizando novamente o backlog
</commit_message>
<xml_diff>
--- a/Backlog-Orchis System.xlsx
+++ b/Backlog-Orchis System.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\OrchisSystems\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272AEB91-CDEE-47F9-833D-6B7E31527685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6012108E-C948-4D6E-A2C8-3CB329DA674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="151">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>ESTIMATIVA(Dias)</t>
+  </si>
+  <si>
+    <t>Estimativa</t>
   </si>
 </sst>
 </file>
@@ -3811,10 +3814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4375,7 +4378,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>52</v>
       </c>
@@ -4410,7 +4413,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>54</v>
       </c>
@@ -4445,7 +4448,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>57</v>
       </c>
@@ -4480,7 +4483,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>59</v>
       </c>
@@ -4515,7 +4518,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>61</v>
       </c>
@@ -4550,7 +4553,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>63</v>
       </c>
@@ -4585,7 +4588,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>65</v>
       </c>
@@ -4620,7 +4623,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>67</v>
       </c>
@@ -4653,9 +4656,14 @@
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-    </row>
-    <row r="25" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>69</v>
       </c>
@@ -4695,7 +4703,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>75</v>
       </c>
@@ -4735,7 +4743,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>77</v>
       </c>
@@ -4775,7 +4783,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>79</v>
       </c>
@@ -4815,7 +4823,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>82</v>
       </c>
@@ -4855,7 +4863,7 @@
         <v>155.66666666666666</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>86</v>
       </c>
@@ -4890,7 +4898,7 @@
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
     </row>
-    <row r="31" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>88</v>
       </c>
@@ -4925,7 +4933,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>90</v>
       </c>

</xml_diff>